<commit_message>
graphing code and new graphs
</commit_message>
<xml_diff>
--- a/results/probability_data_theta_and_phi.xlsx
+++ b/results/probability_data_theta_and_phi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisWiseLocal\GitHub\ZEIT3191-ML-Quantum-Computing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9C02A7-454B-4039-9D32-311C5C88AB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE3CBAF-124C-4693-8876-2F77CE97F2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,28 +304,28 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="R50" sqref="R50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,36 +655,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="29"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="23"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
@@ -721,7 +721,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5">
@@ -769,7 +769,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="6">
         <v>0.3490658503988659</v>
       </c>
@@ -815,7 +815,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="6">
         <v>0.69813170079773179</v>
       </c>
@@ -861,7 +861,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="6">
         <v>1.0471975511965981</v>
       </c>
@@ -907,7 +907,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="6">
         <v>1.396263401595464</v>
       </c>
@@ -953,7 +953,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="6">
         <v>1.74532925199433</v>
       </c>
@@ -999,7 +999,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="6">
         <v>2.0943951023931948</v>
       </c>
@@ -1045,7 +1045,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="6">
         <v>2.4434609527920612</v>
       </c>
@@ -1091,7 +1091,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="6">
         <v>2.7925268031909272</v>
       </c>
@@ -1137,7 +1137,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="7">
         <v>3.1415926535897931</v>
       </c>
@@ -1183,36 +1183,36 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="26"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="29"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="29"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="23"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
@@ -1249,7 +1249,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="24" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="5">
@@ -1287,7 +1287,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="6">
         <v>0.3490658503988659</v>
       </c>
@@ -1323,7 +1323,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="6">
         <v>0.69813170079773179</v>
       </c>
@@ -1359,7 +1359,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="6">
         <v>1.0471975511965981</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="6">
         <v>1.396263401595464</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="6">
         <v>1.74532925199433</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="6">
         <v>2.0943951023931948</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="6">
         <v>2.4434609527920612</v>
       </c>
@@ -1539,7 +1539,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="6">
         <v>2.7925268031909272</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="7">
         <v>3.1415926535897931</v>
       </c>
@@ -1611,36 +1611,36 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="26"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="29"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="29"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="23"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
@@ -1677,496 +1677,396 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="24" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="5">
         <v>0</v>
       </c>
       <c r="C32" s="11">
-        <f t="shared" ref="C32:L32" si="1">ABS(C18-C4)</f>
         <v>1.3900000000000023E-2</v>
       </c>
       <c r="D32" s="8">
-        <f t="shared" si="1"/>
         <v>1.3850000000000029E-2</v>
       </c>
       <c r="E32" s="8">
-        <f t="shared" si="1"/>
         <v>1.2700000000000045E-2</v>
       </c>
       <c r="F32" s="8">
-        <f t="shared" si="1"/>
         <v>1.265000000000005E-2</v>
       </c>
       <c r="G32" s="8">
-        <f t="shared" si="1"/>
         <v>1.1750000000000038E-2</v>
       </c>
       <c r="H32" s="8">
-        <f t="shared" si="1"/>
         <v>1.2850000000000028E-2</v>
       </c>
       <c r="I32" s="8">
-        <f t="shared" si="1"/>
         <v>1.2000000000000011E-2</v>
       </c>
       <c r="J32" s="8">
-        <f t="shared" si="1"/>
         <v>1.1900000000000022E-2</v>
       </c>
       <c r="K32" s="8">
-        <f t="shared" si="1"/>
         <v>1.485000000000003E-2</v>
       </c>
       <c r="L32" s="17">
-        <f t="shared" si="1"/>
         <v>1.2950000000000017E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="6">
         <v>0.31415926535897931</v>
       </c>
       <c r="C33" s="12">
-        <f t="shared" ref="C33:L33" si="2">ABS(C19-C5)</f>
         <v>1.3196310392954103E-2</v>
       </c>
       <c r="D33" s="18">
-        <f t="shared" si="2"/>
         <v>1.0146310392954105E-2</v>
       </c>
       <c r="E33" s="18">
-        <f t="shared" si="2"/>
         <v>7.2463103929540917E-3</v>
       </c>
       <c r="F33" s="18">
-        <f t="shared" si="2"/>
         <v>9.7463103929541495E-3</v>
       </c>
       <c r="G33" s="18">
-        <f t="shared" si="2"/>
         <v>1.1146310392954106E-2</v>
       </c>
       <c r="H33" s="18">
-        <f t="shared" si="2"/>
         <v>7.9963103929541202E-3</v>
       </c>
       <c r="I33" s="18">
-        <f t="shared" si="2"/>
         <v>8.9463103929541266E-3</v>
       </c>
       <c r="J33" s="18">
-        <f t="shared" si="2"/>
         <v>8.8963103929541321E-3</v>
       </c>
       <c r="K33" s="18">
-        <f t="shared" si="2"/>
         <v>1.1246310392954095E-2</v>
       </c>
       <c r="L33" s="19">
-        <f t="shared" si="2"/>
         <v>9.5463103929540605E-3</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="6">
         <v>0.62831853071795862</v>
       </c>
       <c r="C34" s="12">
-        <f t="shared" ref="C34:L34" si="3">ABS(C20-C6)</f>
         <v>1.1272221559489037E-2</v>
       </c>
       <c r="D34" s="18">
-        <f t="shared" si="3"/>
         <v>1.2777784405109127E-3</v>
       </c>
       <c r="E34" s="18">
-        <f t="shared" si="3"/>
         <v>1.8222215594890789E-3</v>
       </c>
       <c r="F34" s="18">
-        <f t="shared" si="3"/>
         <v>7.7222155948908355E-4</v>
       </c>
       <c r="G34" s="18">
-        <f t="shared" si="3"/>
         <v>1.6722215594890955E-3</v>
       </c>
       <c r="H34" s="18">
-        <f t="shared" si="3"/>
         <v>1.9222215594890679E-3</v>
       </c>
       <c r="I34" s="18">
-        <f t="shared" si="3"/>
         <v>1.6777784405109797E-3</v>
       </c>
       <c r="J34" s="18">
-        <f t="shared" si="3"/>
         <v>1.0277784405109402E-3</v>
       </c>
       <c r="K34" s="18">
-        <f t="shared" si="3"/>
         <v>1.8222215594890789E-3</v>
       </c>
       <c r="L34" s="19">
-        <f t="shared" si="3"/>
         <v>3.0222215594890578E-3</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="6">
         <v>0.94247779607693793</v>
       </c>
       <c r="C35" s="12">
-        <f t="shared" ref="C35:L35" si="4">ABS(C21-C7)</f>
         <v>1.8999999999999018E-3</v>
       </c>
       <c r="D35" s="18">
-        <f t="shared" si="4"/>
         <v>8.8500000000001355E-3</v>
       </c>
       <c r="E35" s="18">
-        <f t="shared" si="4"/>
         <v>1.0200000000000098E-2</v>
       </c>
       <c r="F35" s="18">
-        <f t="shared" si="4"/>
         <v>4.350000000000076E-3</v>
       </c>
       <c r="G35" s="18">
-        <f t="shared" si="4"/>
         <v>9.8500000000001364E-3</v>
       </c>
       <c r="H35" s="18">
-        <f t="shared" si="4"/>
         <v>3.9500000000001201E-3</v>
       </c>
       <c r="I35" s="18">
-        <f t="shared" si="4"/>
         <v>1.3050000000000117E-2</v>
       </c>
       <c r="J35" s="18">
-        <f t="shared" si="4"/>
         <v>7.5500000000000567E-3</v>
       </c>
       <c r="K35" s="18">
-        <f t="shared" si="4"/>
         <v>4.450000000000065E-3</v>
       </c>
       <c r="L35" s="19">
-        <f t="shared" si="4"/>
         <v>4.750000000000143E-3</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="6">
         <v>1.256637061435917</v>
       </c>
       <c r="C36" s="12">
-        <f t="shared" ref="C36:L36" si="5">ABS(C22-C8)</f>
         <v>9.5759111665351115E-3</v>
       </c>
       <c r="D36" s="18">
-        <f t="shared" si="5"/>
         <v>1.8075911166535064E-2</v>
       </c>
       <c r="E36" s="18">
-        <f t="shared" si="5"/>
         <v>1.857591116653512E-2</v>
       </c>
       <c r="F36" s="18">
-        <f t="shared" si="5"/>
         <v>2.3275911166535046E-2</v>
       </c>
       <c r="G36" s="18">
-        <f t="shared" si="5"/>
         <v>1.7725911166535102E-2</v>
       </c>
       <c r="H36" s="18">
-        <f t="shared" si="5"/>
         <v>1.5075911166535061E-2</v>
       </c>
       <c r="I36" s="18">
-        <f t="shared" si="5"/>
         <v>1.8625911166535114E-2</v>
       </c>
       <c r="J36" s="18">
-        <f t="shared" si="5"/>
         <v>1.9525911166535015E-2</v>
       </c>
       <c r="K36" s="18">
-        <f t="shared" si="5"/>
         <v>1.6775911166535096E-2</v>
       </c>
       <c r="L36" s="19">
-        <f t="shared" si="5"/>
         <v>1.7325911166535035E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="6">
         <v>1.570796326794897</v>
       </c>
       <c r="C37" s="12">
-        <f t="shared" ref="C37:L37" si="6">ABS(C23-C9)</f>
         <v>3.0524088833465413E-2</v>
       </c>
       <c r="D37" s="18">
-        <f t="shared" si="6"/>
         <v>3.6124088833465406E-2</v>
       </c>
       <c r="E37" s="18">
-        <f t="shared" si="6"/>
         <v>3.0824088833465435E-2</v>
       </c>
       <c r="F37" s="18">
-        <f t="shared" si="6"/>
         <v>2.6374088833465426E-2</v>
       </c>
       <c r="G37" s="18">
-        <f t="shared" si="6"/>
         <v>2.9674088833465451E-2</v>
       </c>
       <c r="H37" s="18">
-        <f t="shared" si="6"/>
         <v>2.7574088833465404E-2</v>
       </c>
       <c r="I37" s="18">
-        <f t="shared" si="6"/>
         <v>2.9374088833465428E-2</v>
       </c>
       <c r="J37" s="18">
-        <f t="shared" si="6"/>
         <v>3.5674088833465456E-2</v>
       </c>
       <c r="K37" s="18">
-        <f t="shared" si="6"/>
         <v>3.0024088833465412E-2</v>
       </c>
       <c r="L37" s="19">
-        <f t="shared" si="6"/>
         <v>3.792408883346543E-2</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="6">
         <v>1.8849555921538761</v>
       </c>
       <c r="C38" s="12">
-        <f t="shared" ref="C38:L38" si="7">ABS(C24-C10)</f>
         <v>3.5149999999999681E-2</v>
       </c>
       <c r="D38" s="18">
-        <f t="shared" si="7"/>
         <v>4.4399999999999662E-2</v>
       </c>
       <c r="E38" s="18">
-        <f t="shared" si="7"/>
         <v>4.3099999999999694E-2</v>
       </c>
       <c r="F38" s="18">
-        <f t="shared" si="7"/>
         <v>3.8949999999999652E-2</v>
       </c>
       <c r="G38" s="18">
-        <f t="shared" si="7"/>
         <v>4.9049999999999649E-2</v>
       </c>
       <c r="H38" s="18">
-        <f t="shared" si="7"/>
         <v>4.2049999999999643E-2</v>
       </c>
       <c r="I38" s="18">
-        <f t="shared" si="7"/>
         <v>4.7299999999999676E-2</v>
       </c>
       <c r="J38" s="18">
-        <f t="shared" si="7"/>
         <v>4.4999999999999651E-2</v>
       </c>
       <c r="K38" s="18">
-        <f t="shared" si="7"/>
         <v>3.9049999999999641E-2</v>
       </c>
       <c r="L38" s="19">
-        <f t="shared" si="7"/>
         <v>3.8399999999999657E-2</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="6">
         <v>2.1991148575128552</v>
       </c>
       <c r="C39" s="12">
-        <f t="shared" ref="C39:L39" si="8">ABS(C25-C11)</f>
         <v>3.642222155948896E-2</v>
       </c>
       <c r="D39" s="18">
-        <f t="shared" si="8"/>
         <v>5.5672221559488949E-2</v>
       </c>
       <c r="E39" s="18">
-        <f t="shared" si="8"/>
         <v>4.8322221559488954E-2</v>
       </c>
       <c r="F39" s="18">
-        <f t="shared" si="8"/>
         <v>5.0522221559488961E-2</v>
       </c>
       <c r="G39" s="18">
-        <f t="shared" si="8"/>
         <v>5.147222155948894E-2</v>
       </c>
       <c r="H39" s="18">
-        <f t="shared" si="8"/>
         <v>5.0172221559488944E-2</v>
       </c>
       <c r="I39" s="18">
-        <f t="shared" si="8"/>
         <v>5.3372221559488953E-2</v>
       </c>
       <c r="J39" s="18">
-        <f t="shared" si="8"/>
         <v>5.1372221559488951E-2</v>
       </c>
       <c r="K39" s="18">
-        <f t="shared" si="8"/>
         <v>4.592222155948894E-2</v>
       </c>
       <c r="L39" s="19">
-        <f t="shared" si="8"/>
         <v>4.7572221559488953E-2</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="6">
         <v>2.513274122871834</v>
       </c>
       <c r="C40" s="12">
-        <f t="shared" ref="C40:L40" si="9">ABS(C26-C12)</f>
         <v>5.0146310392954169E-2</v>
       </c>
       <c r="D40" s="18">
-        <f t="shared" si="9"/>
         <v>5.8096310392954167E-2</v>
       </c>
       <c r="E40" s="18">
-        <f t="shared" si="9"/>
         <v>5.6496310392954177E-2</v>
       </c>
       <c r="F40" s="18">
-        <f t="shared" si="9"/>
         <v>5.7196310392954169E-2</v>
       </c>
       <c r="G40" s="18">
-        <f t="shared" si="9"/>
         <v>5.4196310392954167E-2</v>
       </c>
       <c r="H40" s="18">
-        <f t="shared" si="9"/>
         <v>5.4146310392954172E-2</v>
       </c>
       <c r="I40" s="18">
-        <f t="shared" si="9"/>
         <v>5.5646310392954174E-2</v>
       </c>
       <c r="J40" s="18">
-        <f t="shared" si="9"/>
         <v>5.3096310392954177E-2</v>
       </c>
       <c r="K40" s="18">
-        <f t="shared" si="9"/>
         <v>5.2946310392954166E-2</v>
       </c>
       <c r="L40" s="19">
-        <f t="shared" si="9"/>
         <v>5.4946310392954167E-2</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="7">
         <v>2.8274333882308138</v>
       </c>
       <c r="C41" s="10">
-        <f t="shared" ref="C41:L41" si="10">ABS(C27-C13)</f>
         <v>5.3600000000000002E-2</v>
       </c>
       <c r="D41" s="9">
-        <f t="shared" si="10"/>
         <v>5.1900000000000002E-2</v>
       </c>
       <c r="E41" s="9">
-        <f t="shared" si="10"/>
         <v>5.4100000000000002E-2</v>
       </c>
       <c r="F41" s="9">
-        <f t="shared" si="10"/>
         <v>5.355E-2</v>
       </c>
       <c r="G41" s="9">
-        <f t="shared" si="10"/>
         <v>5.3800000000000001E-2</v>
       </c>
       <c r="H41" s="9">
-        <f t="shared" si="10"/>
         <v>5.1549999999999999E-2</v>
       </c>
       <c r="I41" s="9">
-        <f t="shared" si="10"/>
         <v>5.305E-2</v>
       </c>
       <c r="J41" s="9">
-        <f t="shared" si="10"/>
         <v>5.3850000000000002E-2</v>
       </c>
       <c r="K41" s="9">
-        <f t="shared" si="10"/>
         <v>5.425E-2</v>
       </c>
       <c r="L41" s="20">
-        <f t="shared" si="10"/>
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
+      <c r="A43" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="26"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="29"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="27" t="s">
+      <c r="C44" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="29"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="23"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C45" s="3">
@@ -2201,474 +2101,369 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="24" t="s">
         <v>2</v>
       </c>
       <c r="B46" s="5">
         <v>0</v>
       </c>
       <c r="C46" s="11">
-        <f t="shared" ref="C46:L46" si="11">ABS(C32-C18)</f>
-        <v>0.97219999999999995</v>
+        <v>1.3900000000000023E-2</v>
       </c>
       <c r="D46" s="8">
-        <f t="shared" si="11"/>
-        <v>0.97229999999999994</v>
+        <v>1.3850000000000029E-2</v>
       </c>
       <c r="E46" s="8">
-        <f t="shared" si="11"/>
-        <v>0.97459999999999991</v>
+        <v>1.2700000000000045E-2</v>
       </c>
       <c r="F46" s="8">
-        <f t="shared" si="11"/>
-        <v>0.9746999999999999</v>
+        <v>1.265000000000005E-2</v>
       </c>
       <c r="G46" s="8">
-        <f t="shared" si="11"/>
-        <v>0.97649999999999992</v>
+        <v>1.1750000000000038E-2</v>
       </c>
       <c r="H46" s="8">
-        <f t="shared" si="11"/>
-        <v>0.97429999999999994</v>
+        <v>1.2850000000000028E-2</v>
       </c>
       <c r="I46" s="8">
-        <f t="shared" si="11"/>
-        <v>0.97599999999999998</v>
+        <v>1.2000000000000011E-2</v>
       </c>
       <c r="J46" s="8">
-        <f t="shared" si="11"/>
-        <v>0.97619999999999996</v>
+        <v>1.1900000000000022E-2</v>
       </c>
       <c r="K46" s="8">
-        <f t="shared" si="11"/>
-        <v>0.97029999999999994</v>
+        <v>1.485000000000003E-2</v>
       </c>
       <c r="L46" s="17">
-        <f t="shared" si="11"/>
-        <v>0.97409999999999997</v>
+        <v>1.2950000000000017E-2</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="6">
         <v>0.31415926535897931</v>
       </c>
       <c r="C47" s="12">
-        <f t="shared" ref="C47:L47" si="12">ABS(C33-C19)</f>
-        <v>0.9434536896070459</v>
+        <v>1.3196310392954103E-2</v>
       </c>
       <c r="D47" s="18">
-        <f t="shared" si="12"/>
-        <v>0.94955368960704589</v>
+        <v>1.0146310392954105E-2</v>
       </c>
       <c r="E47" s="18">
-        <f t="shared" si="12"/>
-        <v>0.95535368960704592</v>
+        <v>7.2463103929540917E-3</v>
       </c>
       <c r="F47" s="18">
-        <f t="shared" si="12"/>
-        <v>0.9503536896070458</v>
+        <v>9.7463103929541495E-3</v>
       </c>
       <c r="G47" s="18">
-        <f t="shared" si="12"/>
-        <v>0.94755368960704589</v>
+        <v>1.1146310392954106E-2</v>
       </c>
       <c r="H47" s="18">
-        <f t="shared" si="12"/>
-        <v>0.95385368960704586</v>
+        <v>7.9963103929541202E-3</v>
       </c>
       <c r="I47" s="18">
-        <f t="shared" si="12"/>
-        <v>0.95195368960704585</v>
+        <v>8.9463103929541266E-3</v>
       </c>
       <c r="J47" s="18">
-        <f t="shared" si="12"/>
-        <v>0.95205368960704584</v>
+        <v>8.8963103929541321E-3</v>
       </c>
       <c r="K47" s="18">
-        <f t="shared" si="12"/>
-        <v>0.94735368960704591</v>
+        <v>1.1246310392954095E-2</v>
       </c>
       <c r="L47" s="19">
-        <f t="shared" si="12"/>
-        <v>0.95075368960704598</v>
+        <v>9.5463103929540605E-3</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="6">
         <v>0.62831853071795862</v>
       </c>
       <c r="C48" s="12">
-        <f t="shared" ref="C48:L48" si="13">ABS(C34-C20)</f>
-        <v>0.86047777844051099</v>
+        <v>1.1272221559489037E-2</v>
       </c>
       <c r="D48" s="18">
-        <f t="shared" si="13"/>
-        <v>0.88302222155948906</v>
+        <v>1.2777784405109127E-3</v>
       </c>
       <c r="E48" s="18">
-        <f t="shared" si="13"/>
-        <v>0.8793777784405109</v>
+        <v>1.8222215594890789E-3</v>
       </c>
       <c r="F48" s="18">
-        <f t="shared" si="13"/>
-        <v>0.8814777784405109</v>
+        <v>7.7222155948908355E-4</v>
       </c>
       <c r="G48" s="18">
-        <f t="shared" si="13"/>
-        <v>0.87967777844051087</v>
+        <v>1.6722215594890955E-3</v>
       </c>
       <c r="H48" s="18">
-        <f t="shared" si="13"/>
-        <v>0.87917777844051093</v>
+        <v>1.9222215594890679E-3</v>
       </c>
       <c r="I48" s="18">
-        <f t="shared" si="13"/>
-        <v>0.88302222155948906</v>
+        <v>1.6777784405109797E-3</v>
       </c>
       <c r="J48" s="18">
-        <f t="shared" si="13"/>
-        <v>0.88302222155948906</v>
+        <v>1.0277784405109402E-3</v>
       </c>
       <c r="K48" s="18">
-        <f t="shared" si="13"/>
-        <v>0.8793777784405109</v>
+        <v>1.8222215594890789E-3</v>
       </c>
       <c r="L48" s="19">
-        <f t="shared" si="13"/>
-        <v>0.87697777844051095</v>
+        <v>3.0222215594890578E-3</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="6">
         <v>0.94247779607693793</v>
       </c>
       <c r="C49" s="12">
-        <f t="shared" ref="C49:L49" si="14">ABS(C35-C21)</f>
-        <v>0.74620000000000009</v>
+        <v>1.8999999999999018E-3</v>
       </c>
       <c r="D49" s="18">
-        <f t="shared" si="14"/>
-        <v>0.74999999999999989</v>
+        <v>8.8500000000001355E-3</v>
       </c>
       <c r="E49" s="18">
-        <f t="shared" si="14"/>
-        <v>0.74999999999999989</v>
+        <v>1.0200000000000098E-2</v>
       </c>
       <c r="F49" s="18">
-        <f t="shared" si="14"/>
-        <v>0.74999999999999989</v>
+        <v>4.350000000000076E-3</v>
       </c>
       <c r="G49" s="18">
-        <f t="shared" si="14"/>
-        <v>0.74999999999999989</v>
+        <v>9.8500000000001364E-3</v>
       </c>
       <c r="H49" s="18">
-        <f t="shared" si="14"/>
-        <v>0.74999999999999989</v>
+        <v>3.9500000000001201E-3</v>
       </c>
       <c r="I49" s="18">
-        <f t="shared" si="14"/>
-        <v>0.74999999999999989</v>
+        <v>1.3050000000000117E-2</v>
       </c>
       <c r="J49" s="18">
-        <f t="shared" si="14"/>
-        <v>0.74999999999999989</v>
+        <v>7.5500000000000567E-3</v>
       </c>
       <c r="K49" s="18">
-        <f t="shared" si="14"/>
-        <v>0.74999999999999989</v>
+        <v>4.450000000000065E-3</v>
       </c>
       <c r="L49" s="19">
-        <f t="shared" si="14"/>
-        <v>0.74999999999999989</v>
+        <v>4.750000000000143E-3</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="6">
         <v>1.256637061435917</v>
       </c>
       <c r="C50" s="12">
-        <f t="shared" ref="C50:L50" si="15">ABS(C36-C22)</f>
-        <v>0.58682408883346493</v>
+        <v>9.5759111665351115E-3</v>
       </c>
       <c r="D50" s="18">
-        <f t="shared" si="15"/>
-        <v>0.58682408883346493</v>
+        <v>1.8075911166535064E-2</v>
       </c>
       <c r="E50" s="18">
-        <f t="shared" si="15"/>
-        <v>0.58682408883346493</v>
+        <v>1.857591116653512E-2</v>
       </c>
       <c r="F50" s="18">
-        <f t="shared" si="15"/>
-        <v>0.58682408883346493</v>
+        <v>2.3275911166535046E-2</v>
       </c>
       <c r="G50" s="18">
-        <f t="shared" si="15"/>
-        <v>0.58682408883346493</v>
+        <v>1.7725911166535102E-2</v>
       </c>
       <c r="H50" s="18">
-        <f t="shared" si="15"/>
-        <v>0.58682408883346493</v>
+        <v>1.5075911166535061E-2</v>
       </c>
       <c r="I50" s="18">
-        <f t="shared" si="15"/>
-        <v>0.58682408883346493</v>
+        <v>1.8625911166535114E-2</v>
       </c>
       <c r="J50" s="18">
-        <f t="shared" si="15"/>
-        <v>0.58682408883346493</v>
+        <v>1.9525911166535015E-2</v>
       </c>
       <c r="K50" s="18">
-        <f t="shared" si="15"/>
-        <v>0.58682408883346493</v>
+        <v>1.6775911166535096E-2</v>
       </c>
       <c r="L50" s="19">
-        <f t="shared" si="15"/>
-        <v>0.58682408883346493</v>
+        <v>1.7325911166535035E-2</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="6">
         <v>1.570796326794897</v>
       </c>
       <c r="C51" s="12">
-        <f t="shared" ref="C51:L51" si="16">ABS(C37-C23)</f>
-        <v>0.41317591116653457</v>
+        <v>3.0524088833465413E-2</v>
       </c>
       <c r="D51" s="18">
-        <f t="shared" si="16"/>
-        <v>0.41317591116653457</v>
+        <v>3.6124088833465406E-2</v>
       </c>
       <c r="E51" s="18">
-        <f t="shared" si="16"/>
-        <v>0.41317591116653457</v>
+        <v>3.0824088833465435E-2</v>
       </c>
       <c r="F51" s="18">
-        <f t="shared" si="16"/>
-        <v>0.41317591116653457</v>
+        <v>2.6374088833465426E-2</v>
       </c>
       <c r="G51" s="18">
-        <f t="shared" si="16"/>
-        <v>0.41317591116653457</v>
+        <v>2.9674088833465451E-2</v>
       </c>
       <c r="H51" s="18">
-        <f t="shared" si="16"/>
-        <v>0.41317591116653457</v>
+        <v>2.7574088833465404E-2</v>
       </c>
       <c r="I51" s="18">
-        <f t="shared" si="16"/>
-        <v>0.41317591116653457</v>
+        <v>2.9374088833465428E-2</v>
       </c>
       <c r="J51" s="18">
-        <f t="shared" si="16"/>
-        <v>0.41317591116653457</v>
+        <v>3.5674088833465456E-2</v>
       </c>
       <c r="K51" s="18">
-        <f t="shared" si="16"/>
-        <v>0.41317591116653457</v>
+        <v>3.0024088833465412E-2</v>
       </c>
       <c r="L51" s="19">
-        <f t="shared" si="16"/>
-        <v>0.41317591116653457</v>
+        <v>3.792408883346543E-2</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
+      <c r="A52" s="25"/>
       <c r="B52" s="6">
         <v>1.8849555921538761</v>
       </c>
       <c r="C52" s="12">
-        <f t="shared" ref="C52:L52" si="17">ABS(C38-C24)</f>
-        <v>0.25000000000000033</v>
+        <v>3.5149999999999681E-2</v>
       </c>
       <c r="D52" s="18">
-        <f t="shared" si="17"/>
-        <v>0.25000000000000033</v>
+        <v>4.4399999999999662E-2</v>
       </c>
       <c r="E52" s="18">
-        <f t="shared" si="17"/>
-        <v>0.25000000000000033</v>
+        <v>4.3099999999999694E-2</v>
       </c>
       <c r="F52" s="18">
-        <f t="shared" si="17"/>
-        <v>0.25000000000000033</v>
+        <v>3.8949999999999652E-2</v>
       </c>
       <c r="G52" s="18">
-        <f t="shared" si="17"/>
-        <v>0.25000000000000033</v>
+        <v>4.9049999999999649E-2</v>
       </c>
       <c r="H52" s="18">
-        <f t="shared" si="17"/>
-        <v>0.25000000000000033</v>
+        <v>4.2049999999999643E-2</v>
       </c>
       <c r="I52" s="18">
-        <f t="shared" si="17"/>
-        <v>0.25000000000000033</v>
+        <v>4.7299999999999676E-2</v>
       </c>
       <c r="J52" s="18">
-        <f t="shared" si="17"/>
-        <v>0.25000000000000033</v>
+        <v>4.4999999999999651E-2</v>
       </c>
       <c r="K52" s="18">
-        <f t="shared" si="17"/>
-        <v>0.25000000000000033</v>
+        <v>3.9049999999999641E-2</v>
       </c>
       <c r="L52" s="19">
-        <f t="shared" si="17"/>
-        <v>0.25000000000000033</v>
+        <v>3.8399999999999657E-2</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="6">
         <v>2.1991148575128552</v>
       </c>
       <c r="C53" s="12">
-        <f t="shared" ref="C53:L53" si="18">ABS(C39-C25)</f>
-        <v>0.11697777844051105</v>
+        <v>3.642222155948896E-2</v>
       </c>
       <c r="D53" s="18">
-        <f t="shared" si="18"/>
-        <v>0.11697777844051105</v>
+        <v>5.5672221559488949E-2</v>
       </c>
       <c r="E53" s="18">
-        <f t="shared" si="18"/>
-        <v>0.11697777844051105</v>
+        <v>4.8322221559488954E-2</v>
       </c>
       <c r="F53" s="18">
-        <f t="shared" si="18"/>
-        <v>0.11697777844051105</v>
+        <v>5.0522221559488961E-2</v>
       </c>
       <c r="G53" s="18">
-        <f t="shared" si="18"/>
-        <v>0.11697777844051105</v>
+        <v>5.147222155948894E-2</v>
       </c>
       <c r="H53" s="18">
-        <f t="shared" si="18"/>
-        <v>0.11697777844051105</v>
+        <v>5.0172221559488944E-2</v>
       </c>
       <c r="I53" s="18">
-        <f t="shared" si="18"/>
-        <v>0.11697777844051105</v>
+        <v>5.3372221559488953E-2</v>
       </c>
       <c r="J53" s="18">
-        <f t="shared" si="18"/>
-        <v>0.11697777844051105</v>
+        <v>5.1372221559488951E-2</v>
       </c>
       <c r="K53" s="18">
-        <f t="shared" si="18"/>
-        <v>0.11697777844051105</v>
+        <v>4.592222155948894E-2</v>
       </c>
       <c r="L53" s="19">
-        <f t="shared" si="18"/>
-        <v>0.11697777844051105</v>
+        <v>4.7572221559488953E-2</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
+      <c r="A54" s="25"/>
       <c r="B54" s="6">
         <v>2.513274122871834</v>
       </c>
       <c r="C54" s="12">
-        <f t="shared" ref="C54:L54" si="19">ABS(C40-C26)</f>
-        <v>3.0153689607045828E-2</v>
+        <v>5.0146310392954169E-2</v>
       </c>
       <c r="D54" s="18">
-        <f t="shared" si="19"/>
-        <v>3.0153689607045828E-2</v>
+        <v>5.8096310392954167E-2</v>
       </c>
       <c r="E54" s="18">
-        <f t="shared" si="19"/>
-        <v>3.0153689607045828E-2</v>
+        <v>5.6496310392954177E-2</v>
       </c>
       <c r="F54" s="18">
-        <f t="shared" si="19"/>
-        <v>3.0153689607045828E-2</v>
+        <v>5.7196310392954169E-2</v>
       </c>
       <c r="G54" s="18">
-        <f t="shared" si="19"/>
-        <v>3.0153689607045828E-2</v>
+        <v>5.4196310392954167E-2</v>
       </c>
       <c r="H54" s="18">
-        <f t="shared" si="19"/>
-        <v>3.0153689607045828E-2</v>
+        <v>5.4146310392954172E-2</v>
       </c>
       <c r="I54" s="18">
-        <f t="shared" si="19"/>
-        <v>3.0153689607045828E-2</v>
+        <v>5.5646310392954174E-2</v>
       </c>
       <c r="J54" s="18">
-        <f t="shared" si="19"/>
-        <v>3.0153689607045828E-2</v>
+        <v>5.3096310392954177E-2</v>
       </c>
       <c r="K54" s="18">
-        <f t="shared" si="19"/>
-        <v>3.0153689607045828E-2</v>
+        <v>5.2946310392954166E-2</v>
       </c>
       <c r="L54" s="19">
-        <f t="shared" si="19"/>
-        <v>3.0153689607045828E-2</v>
+        <v>5.4946310392954167E-2</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="7">
         <v>2.8274333882308138</v>
       </c>
       <c r="C55" s="10">
-        <f t="shared" ref="C55:L55" si="20">ABS(C41-C27)</f>
-        <v>0</v>
+        <v>5.3600000000000002E-2</v>
       </c>
       <c r="D55" s="9">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.1900000000000002E-2</v>
       </c>
       <c r="E55" s="9">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.4100000000000002E-2</v>
       </c>
       <c r="F55" s="9">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.355E-2</v>
       </c>
       <c r="G55" s="9">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.3800000000000001E-2</v>
       </c>
       <c r="H55" s="9">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.1549999999999999E-2</v>
       </c>
       <c r="I55" s="9">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.305E-2</v>
       </c>
       <c r="J55" s="9">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.3850000000000002E-2</v>
       </c>
       <c r="K55" s="9">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.425E-2</v>
       </c>
       <c r="L55" s="20">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>5.2499999999999998E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C44:L44"/>
-    <mergeCell ref="A46:A55"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="C30:L30"/>
-    <mergeCell ref="A32:A41"/>
     <mergeCell ref="A4:A13"/>
     <mergeCell ref="A43:L43"/>
     <mergeCell ref="C2:L2"/>
@@ -2676,6 +2471,11 @@
     <mergeCell ref="A15:L15"/>
     <mergeCell ref="C16:L16"/>
     <mergeCell ref="A18:A27"/>
+    <mergeCell ref="C44:L44"/>
+    <mergeCell ref="A46:A55"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="C30:L30"/>
+    <mergeCell ref="A32:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>